<commit_message>
Se finalizan 3 transacciones de saldos y movimientos
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/consultas/detalleproductos/ConsultaDetalleCuentaDeposito.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/consultas/detalleproductos/ConsultaDetalleCuentaDeposito.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="45">
   <si>
     <t>ID</t>
   </si>
@@ -67,52 +67,43 @@
     <t>1037655531</t>
   </si>
   <si>
+    <t>userrobot3</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>4321</t>
+  </si>
+  <si>
+    <t>Acierto</t>
+  </si>
+  <si>
+    <t>000</t>
+  </si>
+  <si>
+    <t>0369</t>
+  </si>
+  <si>
+    <t>NO ERROR</t>
+  </si>
+  <si>
+    <t>bolp</t>
+  </si>
+  <si>
+    <t>ACTIVO</t>
+  </si>
+  <si>
+    <t>Corriente</t>
+  </si>
+  <si>
+    <t>406-101390-08</t>
+  </si>
+  <si>
+    <t>zrediseño12</t>
+  </si>
+  <si>
     <t>userqa10</t>
-  </si>
-  <si>
-    <t>1234</t>
-  </si>
-  <si>
-    <t>4321</t>
-  </si>
-  <si>
-    <t>Acierto</t>
-  </si>
-  <si>
-    <t>000</t>
-  </si>
-  <si>
-    <t>0369</t>
-  </si>
-  <si>
-    <t>NO ERROR</t>
-  </si>
-  <si>
-    <t>bolp</t>
-  </si>
-  <si>
-    <t>ACTIVO</t>
-  </si>
-  <si>
-    <t>Cuenta de Ahorro</t>
-  </si>
-  <si>
-    <t>406-740100-05</t>
-  </si>
-  <si>
-    <t>zrediseño12</t>
-  </si>
-  <si>
-    <t>Prestamo Personal Ta;Prestamo Personal Ta</t>
-  </si>
-  <si>
-    <t>29281005510;29281023970</t>
-  </si>
-  <si>
-    <t>Personal Visa;Personal Mastercard</t>
-  </si>
-  <si>
-    <t>*6401;*5365</t>
   </si>
   <si>
     <t>Orientacion</t>
@@ -206,7 +197,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -214,13 +205,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -241,8 +225,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -251,9 +273,53 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -272,81 +338,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -375,61 +366,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -441,7 +534,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -453,109 +546,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -584,17 +575,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -604,30 +591,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -649,11 +612,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -673,160 +649,175 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1166,8 +1157,8 @@
   <sheetPr/>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
@@ -1313,8 +1304,8 @@
   <sheetPr/>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
@@ -1408,12 +1399,8 @@
       <c r="L2" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="5"/>
@@ -1461,7 +1448,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
@@ -1529,7 +1516,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>17</v>
@@ -1555,12 +1542,8 @@
       <c r="L2" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>31</v>
-      </c>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="5"/>
@@ -1621,16 +1604,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
         <v>32</v>
-      </c>
-      <c r="B1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1638,50 +1621,50 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
         <v>39</v>
-      </c>
-      <c r="B3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>